<commit_message>
Update IP - EX 40 - Plus Super exercicio II (Anexo).xlsx
Exercicio
</commit_message>
<xml_diff>
--- a/Materia_2-PowerBi/IP - EX 40 - Plus Super exercicio II (Anexo).xlsx
+++ b/Materia_2-PowerBi/IP - EX 40 - Plus Super exercicio II (Anexo).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bianc\4)DNC\Repositorio\DNC_DataScience\Materia_2-PowerBi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9CC9976-1950-4B29-9B8E-89F264D7BAEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBCA4899-FC2F-4C46-ADBA-205834E39E59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -654,7 +654,7 @@
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -805,6 +805,7 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -812,7 +813,37 @@
     <cellStyle name="SAPBEXfilterDrill" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Vírgula 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1252,8 +1283,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:S138"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19:J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1503,6 +1534,9 @@
       <c r="Q17" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="R17" s="64">
+        <v>0.15</v>
+      </c>
       <c r="S17" s="8"/>
     </row>
     <row r="18" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1551,7 +1585,10 @@
         <v>120.16242246311212</v>
       </c>
       <c r="H19" s="63"/>
-      <c r="I19" s="51"/>
+      <c r="I19" s="51" t="str">
+        <f>UPPER(IF(OR(G19&gt;E19+C19*(1+R17)),"Reprovado",IF(AND(G19&gt;E19-C19,G19&lt;E19+C19),"Aprovado","Retrabalho")))</f>
+        <v>APROVADO</v>
+      </c>
       <c r="J19" s="52"/>
       <c r="N19" s="12"/>
       <c r="O19" s="9"/>
@@ -1576,7 +1613,10 @@
         <v>120.56079525991738</v>
       </c>
       <c r="H20" s="50"/>
-      <c r="I20" s="51"/>
+      <c r="I20" s="51" t="str">
+        <f t="shared" ref="I20:I83" si="0">UPPER(IF(OR(G20&gt;E20+C20*(1+R18)),"Reprovado",IF(AND(G20&gt;E20-C20,G20&lt;E20+C20),"Aprovado","Retrabalho")))</f>
+        <v>APROVADO</v>
+      </c>
       <c r="J20" s="52"/>
     </row>
     <row r="21" spans="2:19" x14ac:dyDescent="0.25">
@@ -1595,7 +1635,10 @@
         <v>125.51923861930177</v>
       </c>
       <c r="H21" s="50"/>
-      <c r="I21" s="51"/>
+      <c r="I21" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>REPROVADO</v>
+      </c>
       <c r="J21" s="52"/>
       <c r="N21" s="13" t="s">
         <v>18</v>
@@ -1622,7 +1665,10 @@
         <v>122.80213508162171</v>
       </c>
       <c r="H22" s="50"/>
-      <c r="I22" s="51"/>
+      <c r="I22" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>REPROVADO</v>
+      </c>
       <c r="J22" s="52"/>
       <c r="N22" s="16" t="s">
         <v>19</v>
@@ -1649,7 +1695,10 @@
         <v>125.75602416248303</v>
       </c>
       <c r="H23" s="50"/>
-      <c r="I23" s="51"/>
+      <c r="I23" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>REPROVADO</v>
+      </c>
       <c r="J23" s="52"/>
       <c r="N23" s="16" t="s">
         <v>15</v>
@@ -1676,7 +1725,10 @@
         <v>122.40175711815594</v>
       </c>
       <c r="H24" s="50"/>
-      <c r="I24" s="51"/>
+      <c r="I24" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>REPROVADO</v>
+      </c>
       <c r="J24" s="52"/>
       <c r="N24" s="24" t="s">
         <v>21</v>
@@ -1703,7 +1755,10 @@
         <v>120.14982908470529</v>
       </c>
       <c r="H25" s="50"/>
-      <c r="I25" s="51"/>
+      <c r="I25" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>APROVADO</v>
+      </c>
       <c r="J25" s="52"/>
       <c r="N25" s="24" t="s">
         <v>22</v>
@@ -1730,7 +1785,10 @@
         <v>123.35264481565088</v>
       </c>
       <c r="H26" s="50"/>
-      <c r="I26" s="51"/>
+      <c r="I26" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>REPROVADO</v>
+      </c>
       <c r="J26" s="52"/>
       <c r="N26" s="19" t="s">
         <v>14</v>
@@ -1757,7 +1815,10 @@
         <v>124.65205362043356</v>
       </c>
       <c r="H27" s="50"/>
-      <c r="I27" s="51"/>
+      <c r="I27" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>REPROVADO</v>
+      </c>
       <c r="J27" s="52"/>
     </row>
     <row r="28" spans="2:19" x14ac:dyDescent="0.25">
@@ -1776,7 +1837,10 @@
         <v>123.34633710714813</v>
       </c>
       <c r="H28" s="50"/>
-      <c r="I28" s="51"/>
+      <c r="I28" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>REPROVADO</v>
+      </c>
       <c r="J28" s="52"/>
     </row>
     <row r="29" spans="2:19" x14ac:dyDescent="0.25">
@@ -1795,7 +1859,10 @@
         <v>123.06833036749381</v>
       </c>
       <c r="H29" s="50"/>
-      <c r="I29" s="51"/>
+      <c r="I29" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>REPROVADO</v>
+      </c>
       <c r="J29" s="52"/>
     </row>
     <row r="30" spans="2:19" x14ac:dyDescent="0.25">
@@ -1814,7 +1881,10 @@
         <v>119.52885589452302</v>
       </c>
       <c r="H30" s="50"/>
-      <c r="I30" s="51"/>
+      <c r="I30" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>APROVADO</v>
+      </c>
       <c r="J30" s="52"/>
     </row>
     <row r="31" spans="2:19" x14ac:dyDescent="0.25">
@@ -1833,7 +1903,10 @@
         <v>119.32876490622201</v>
       </c>
       <c r="H31" s="50"/>
-      <c r="I31" s="51"/>
+      <c r="I31" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>APROVADO</v>
+      </c>
       <c r="J31" s="52"/>
     </row>
     <row r="32" spans="2:19" x14ac:dyDescent="0.25">
@@ -1852,7 +1925,10 @@
         <v>120.60923383150566</v>
       </c>
       <c r="H32" s="50"/>
-      <c r="I32" s="51"/>
+      <c r="I32" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>APROVADO</v>
+      </c>
       <c r="J32" s="52"/>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.25">
@@ -1871,7 +1947,10 @@
         <v>124.84765366680351</v>
       </c>
       <c r="H33" s="50"/>
-      <c r="I33" s="51"/>
+      <c r="I33" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>REPROVADO</v>
+      </c>
       <c r="J33" s="52"/>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.25">
@@ -1890,7 +1969,10 @@
         <v>122.54782615795668</v>
       </c>
       <c r="H34" s="50"/>
-      <c r="I34" s="51"/>
+      <c r="I34" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>REPROVADO</v>
+      </c>
       <c r="J34" s="52"/>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.25">
@@ -1909,7 +1991,10 @@
         <v>122.95087840593206</v>
       </c>
       <c r="H35" s="50"/>
-      <c r="I35" s="51"/>
+      <c r="I35" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>REPROVADO</v>
+      </c>
       <c r="J35" s="52"/>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.25">
@@ -1928,7 +2013,10 @@
         <v>119.24467011202594</v>
       </c>
       <c r="H36" s="50"/>
-      <c r="I36" s="51"/>
+      <c r="I36" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>APROVADO</v>
+      </c>
       <c r="J36" s="52"/>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.25">
@@ -1947,7 +2035,10 @@
         <v>118.11115066337196</v>
       </c>
       <c r="H37" s="50"/>
-      <c r="I37" s="51"/>
+      <c r="I37" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>RETRABALHO</v>
+      </c>
       <c r="J37" s="52"/>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.25">
@@ -1966,7 +2057,10 @@
         <v>121.98013917845581</v>
       </c>
       <c r="H38" s="50"/>
-      <c r="I38" s="51"/>
+      <c r="I38" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>REPROVADO</v>
+      </c>
       <c r="J38" s="52"/>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.25">
@@ -1985,7 +2079,10 @@
         <v>118.82037315849256</v>
       </c>
       <c r="H39" s="50"/>
-      <c r="I39" s="51"/>
+      <c r="I39" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>APROVADO</v>
+      </c>
       <c r="J39" s="52"/>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.25">
@@ -2004,7 +2101,10 @@
         <v>118.72661573724687</v>
       </c>
       <c r="H40" s="50"/>
-      <c r="I40" s="51"/>
+      <c r="I40" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>APROVADO</v>
+      </c>
       <c r="J40" s="52"/>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.25">
@@ -2023,7 +2123,10 @@
         <v>121.02773658333982</v>
       </c>
       <c r="H41" s="50"/>
-      <c r="I41" s="51"/>
+      <c r="I41" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>APROVADO</v>
+      </c>
       <c r="J41" s="52"/>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.25">
@@ -2042,7 +2145,10 @@
         <v>122.06299263416956</v>
       </c>
       <c r="H42" s="50"/>
-      <c r="I42" s="51"/>
+      <c r="I42" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>REPROVADO</v>
+      </c>
       <c r="J42" s="52"/>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.25">
@@ -2061,7 +2167,10 @@
         <v>120.83891933584739</v>
       </c>
       <c r="H43" s="50"/>
-      <c r="I43" s="51"/>
+      <c r="I43" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>APROVADO</v>
+      </c>
       <c r="J43" s="52"/>
     </row>
     <row r="44" spans="2:10" x14ac:dyDescent="0.25">
@@ -2080,7 +2189,10 @@
         <v>123.13798728129014</v>
       </c>
       <c r="H44" s="50"/>
-      <c r="I44" s="51"/>
+      <c r="I44" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>REPROVADO</v>
+      </c>
       <c r="J44" s="52"/>
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.25">
@@ -2099,7 +2211,10 @@
         <v>121.03638342749713</v>
       </c>
       <c r="H45" s="50"/>
-      <c r="I45" s="51"/>
+      <c r="I45" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>APROVADO</v>
+      </c>
       <c r="J45" s="52"/>
     </row>
     <row r="46" spans="2:10" x14ac:dyDescent="0.25">
@@ -2118,7 +2233,10 @@
         <v>121.83896058110926</v>
       </c>
       <c r="H46" s="50"/>
-      <c r="I46" s="51"/>
+      <c r="I46" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>REPROVADO</v>
+      </c>
       <c r="J46" s="52"/>
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.25">
@@ -2137,7 +2255,10 @@
         <v>124.85280453514535</v>
       </c>
       <c r="H47" s="50"/>
-      <c r="I47" s="51"/>
+      <c r="I47" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>REPROVADO</v>
+      </c>
       <c r="J47" s="52"/>
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.25">
@@ -2156,7 +2277,10 @@
         <v>119.14448450639033</v>
       </c>
       <c r="H48" s="50"/>
-      <c r="I48" s="51"/>
+      <c r="I48" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>APROVADO</v>
+      </c>
       <c r="J48" s="52"/>
     </row>
     <row r="49" spans="2:10" x14ac:dyDescent="0.25">
@@ -2175,7 +2299,10 @@
         <v>118.07563132881678</v>
       </c>
       <c r="H49" s="50"/>
-      <c r="I49" s="51"/>
+      <c r="I49" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>RETRABALHO</v>
+      </c>
       <c r="J49" s="52"/>
     </row>
     <row r="50" spans="2:10" x14ac:dyDescent="0.25">
@@ -2194,7 +2321,10 @@
         <v>120.04892138517866</v>
       </c>
       <c r="H50" s="50"/>
-      <c r="I50" s="51"/>
+      <c r="I50" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>APROVADO</v>
+      </c>
       <c r="J50" s="52"/>
     </row>
     <row r="51" spans="2:10" x14ac:dyDescent="0.25">
@@ -2213,7 +2343,10 @@
         <v>122.89894048906612</v>
       </c>
       <c r="H51" s="50"/>
-      <c r="I51" s="51"/>
+      <c r="I51" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>REPROVADO</v>
+      </c>
       <c r="J51" s="52"/>
     </row>
     <row r="52" spans="2:10" x14ac:dyDescent="0.25">
@@ -2232,7 +2365,10 @@
         <v>118.08323905389796</v>
       </c>
       <c r="H52" s="50"/>
-      <c r="I52" s="51"/>
+      <c r="I52" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>RETRABALHO</v>
+      </c>
       <c r="J52" s="52"/>
     </row>
     <row r="53" spans="2:10" x14ac:dyDescent="0.25">
@@ -2251,7 +2387,10 @@
         <v>122.16640702877247</v>
       </c>
       <c r="H53" s="50"/>
-      <c r="I53" s="51"/>
+      <c r="I53" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>REPROVADO</v>
+      </c>
       <c r="J53" s="52"/>
     </row>
     <row r="54" spans="2:10" x14ac:dyDescent="0.25">
@@ -2270,7 +2409,10 @@
         <v>118.10375234825058</v>
       </c>
       <c r="H54" s="50"/>
-      <c r="I54" s="51"/>
+      <c r="I54" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>RETRABALHO</v>
+      </c>
       <c r="J54" s="52"/>
     </row>
     <row r="55" spans="2:10" x14ac:dyDescent="0.25">
@@ -2289,7 +2431,10 @@
         <v>123.63711667206275</v>
       </c>
       <c r="H55" s="50"/>
-      <c r="I55" s="51"/>
+      <c r="I55" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>REPROVADO</v>
+      </c>
       <c r="J55" s="52"/>
     </row>
     <row r="56" spans="2:10" x14ac:dyDescent="0.25">
@@ -2308,7 +2453,10 @@
         <v>123.98003799662258</v>
       </c>
       <c r="H56" s="50"/>
-      <c r="I56" s="51"/>
+      <c r="I56" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>REPROVADO</v>
+      </c>
       <c r="J56" s="52"/>
     </row>
     <row r="57" spans="2:10" x14ac:dyDescent="0.25">
@@ -2327,7 +2475,10 @@
         <v>120.34286970819676</v>
       </c>
       <c r="H57" s="50"/>
-      <c r="I57" s="51"/>
+      <c r="I57" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>APROVADO</v>
+      </c>
       <c r="J57" s="52"/>
     </row>
     <row r="58" spans="2:10" x14ac:dyDescent="0.25">
@@ -2346,7 +2497,10 @@
         <v>118.90245573314817</v>
       </c>
       <c r="H58" s="50"/>
-      <c r="I58" s="51"/>
+      <c r="I58" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>APROVADO</v>
+      </c>
       <c r="J58" s="52"/>
     </row>
     <row r="59" spans="2:10" x14ac:dyDescent="0.25">
@@ -2365,7 +2519,10 @@
         <v>120.41025352546109</v>
       </c>
       <c r="H59" s="50"/>
-      <c r="I59" s="51"/>
+      <c r="I59" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>APROVADO</v>
+      </c>
       <c r="J59" s="52"/>
     </row>
     <row r="60" spans="2:10" x14ac:dyDescent="0.25">
@@ -2384,7 +2541,10 @@
         <v>125.36199841669726</v>
       </c>
       <c r="H60" s="50"/>
-      <c r="I60" s="51"/>
+      <c r="I60" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>REPROVADO</v>
+      </c>
       <c r="J60" s="52"/>
     </row>
     <row r="61" spans="2:10" x14ac:dyDescent="0.25">
@@ -2403,7 +2563,10 @@
         <v>119.07991526711025</v>
       </c>
       <c r="H61" s="50"/>
-      <c r="I61" s="51"/>
+      <c r="I61" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>APROVADO</v>
+      </c>
       <c r="J61" s="52"/>
     </row>
     <row r="62" spans="2:10" x14ac:dyDescent="0.25">
@@ -2422,7 +2585,10 @@
         <v>118.85711760832687</v>
       </c>
       <c r="H62" s="50"/>
-      <c r="I62" s="51"/>
+      <c r="I62" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>APROVADO</v>
+      </c>
       <c r="J62" s="52"/>
     </row>
     <row r="63" spans="2:10" x14ac:dyDescent="0.25">
@@ -2441,7 +2607,10 @@
         <v>119.19750941231533</v>
       </c>
       <c r="H63" s="50"/>
-      <c r="I63" s="51"/>
+      <c r="I63" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>APROVADO</v>
+      </c>
       <c r="J63" s="52"/>
     </row>
     <row r="64" spans="2:10" x14ac:dyDescent="0.25">
@@ -2460,7 +2629,10 @@
         <v>124.2925032823488</v>
       </c>
       <c r="H64" s="50"/>
-      <c r="I64" s="51"/>
+      <c r="I64" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>REPROVADO</v>
+      </c>
       <c r="J64" s="52"/>
     </row>
     <row r="65" spans="2:10" x14ac:dyDescent="0.25">
@@ -2479,7 +2651,10 @@
         <v>118.70634209083708</v>
       </c>
       <c r="H65" s="50"/>
-      <c r="I65" s="51"/>
+      <c r="I65" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>APROVADO</v>
+      </c>
       <c r="J65" s="52"/>
     </row>
     <row r="66" spans="2:10" x14ac:dyDescent="0.25">
@@ -2498,7 +2673,10 @@
         <v>124.25647807416786</v>
       </c>
       <c r="H66" s="50"/>
-      <c r="I66" s="51"/>
+      <c r="I66" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>REPROVADO</v>
+      </c>
       <c r="J66" s="52"/>
     </row>
     <row r="67" spans="2:10" x14ac:dyDescent="0.25">
@@ -2517,7 +2695,10 @@
         <v>122.0036999861984</v>
       </c>
       <c r="H67" s="50"/>
-      <c r="I67" s="51"/>
+      <c r="I67" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>REPROVADO</v>
+      </c>
       <c r="J67" s="52"/>
     </row>
     <row r="68" spans="2:10" x14ac:dyDescent="0.25">
@@ -2536,7 +2717,10 @@
         <v>123.3310747774226</v>
       </c>
       <c r="H68" s="50"/>
-      <c r="I68" s="51"/>
+      <c r="I68" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>REPROVADO</v>
+      </c>
       <c r="J68" s="52"/>
     </row>
     <row r="69" spans="2:10" x14ac:dyDescent="0.25">
@@ -2555,7 +2739,10 @@
         <v>121.21537477520035</v>
       </c>
       <c r="H69" s="50"/>
-      <c r="I69" s="51"/>
+      <c r="I69" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>APROVADO</v>
+      </c>
       <c r="J69" s="52"/>
     </row>
     <row r="70" spans="2:10" x14ac:dyDescent="0.25">
@@ -2574,7 +2761,10 @@
         <v>122.84352998632018</v>
       </c>
       <c r="H70" s="50"/>
-      <c r="I70" s="51"/>
+      <c r="I70" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>REPROVADO</v>
+      </c>
       <c r="J70" s="52"/>
     </row>
     <row r="71" spans="2:10" x14ac:dyDescent="0.25">
@@ -2593,7 +2783,10 @@
         <v>120.49242285320854</v>
       </c>
       <c r="H71" s="50"/>
-      <c r="I71" s="51"/>
+      <c r="I71" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>APROVADO</v>
+      </c>
       <c r="J71" s="52"/>
     </row>
     <row r="72" spans="2:10" x14ac:dyDescent="0.25">
@@ -2612,7 +2805,10 @@
         <v>119.48506491998208</v>
       </c>
       <c r="H72" s="50"/>
-      <c r="I72" s="51"/>
+      <c r="I72" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>APROVADO</v>
+      </c>
       <c r="J72" s="52"/>
     </row>
     <row r="73" spans="2:10" x14ac:dyDescent="0.25">
@@ -2631,7 +2827,10 @@
         <v>123.78438632741496</v>
       </c>
       <c r="H73" s="50"/>
-      <c r="I73" s="51"/>
+      <c r="I73" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>REPROVADO</v>
+      </c>
       <c r="J73" s="52"/>
     </row>
     <row r="74" spans="2:10" x14ac:dyDescent="0.25">
@@ -2650,7 +2849,10 @@
         <v>123.50330516583304</v>
       </c>
       <c r="H74" s="50"/>
-      <c r="I74" s="51"/>
+      <c r="I74" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>REPROVADO</v>
+      </c>
       <c r="J74" s="52"/>
     </row>
     <row r="75" spans="2:10" x14ac:dyDescent="0.25">
@@ -2669,7 +2871,10 @@
         <v>118.64240604382488</v>
       </c>
       <c r="H75" s="50"/>
-      <c r="I75" s="51"/>
+      <c r="I75" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>APROVADO</v>
+      </c>
       <c r="J75" s="52"/>
     </row>
     <row r="76" spans="2:10" x14ac:dyDescent="0.25">
@@ -2688,7 +2893,10 @@
         <v>120.25088068186345</v>
       </c>
       <c r="H76" s="50"/>
-      <c r="I76" s="51"/>
+      <c r="I76" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>APROVADO</v>
+      </c>
       <c r="J76" s="52"/>
     </row>
     <row r="77" spans="2:10" x14ac:dyDescent="0.25">
@@ -2707,7 +2915,10 @@
         <v>121.19738202474859</v>
       </c>
       <c r="H77" s="50"/>
-      <c r="I77" s="51"/>
+      <c r="I77" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>APROVADO</v>
+      </c>
       <c r="J77" s="52"/>
     </row>
     <row r="78" spans="2:10" x14ac:dyDescent="0.25">
@@ -2726,7 +2937,10 @@
         <v>120.49359507687939</v>
       </c>
       <c r="H78" s="50"/>
-      <c r="I78" s="51"/>
+      <c r="I78" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>APROVADO</v>
+      </c>
       <c r="J78" s="52"/>
     </row>
     <row r="79" spans="2:10" x14ac:dyDescent="0.25">
@@ -2745,7 +2959,10 @@
         <v>125.70483352770094</v>
       </c>
       <c r="H79" s="50"/>
-      <c r="I79" s="51"/>
+      <c r="I79" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>REPROVADO</v>
+      </c>
       <c r="J79" s="52"/>
     </row>
     <row r="80" spans="2:10" x14ac:dyDescent="0.25">
@@ -2764,7 +2981,10 @@
         <v>118.03253934464257</v>
       </c>
       <c r="H80" s="50"/>
-      <c r="I80" s="51"/>
+      <c r="I80" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>RETRABALHO</v>
+      </c>
       <c r="J80" s="52"/>
     </row>
     <row r="81" spans="2:10" x14ac:dyDescent="0.25">
@@ -2783,7 +3003,10 @@
         <v>122.72249440357723</v>
       </c>
       <c r="H81" s="50"/>
-      <c r="I81" s="51"/>
+      <c r="I81" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>REPROVADO</v>
+      </c>
       <c r="J81" s="52"/>
     </row>
     <row r="82" spans="2:10" x14ac:dyDescent="0.25">
@@ -2802,7 +3025,10 @@
         <v>122.59257484555934</v>
       </c>
       <c r="H82" s="50"/>
-      <c r="I82" s="51"/>
+      <c r="I82" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>REPROVADO</v>
+      </c>
       <c r="J82" s="52"/>
     </row>
     <row r="83" spans="2:10" x14ac:dyDescent="0.25">
@@ -2821,7 +3047,10 @@
         <v>121.08341251105658</v>
       </c>
       <c r="H83" s="50"/>
-      <c r="I83" s="51"/>
+      <c r="I83" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>APROVADO</v>
+      </c>
       <c r="J83" s="52"/>
     </row>
     <row r="84" spans="2:10" x14ac:dyDescent="0.25">
@@ -2840,7 +3069,10 @@
         <v>124.66393189791428</v>
       </c>
       <c r="H84" s="50"/>
-      <c r="I84" s="51"/>
+      <c r="I84" s="51" t="str">
+        <f t="shared" ref="I84:I138" si="1">UPPER(IF(OR(G84&gt;E84+C84*(1+R82)),"Reprovado",IF(AND(G84&gt;E84-C84,G84&lt;E84+C84),"Aprovado","Retrabalho")))</f>
+        <v>REPROVADO</v>
+      </c>
       <c r="J84" s="52"/>
     </row>
     <row r="85" spans="2:10" x14ac:dyDescent="0.25">
@@ -2859,7 +3091,10 @@
         <v>125.33388907360646</v>
       </c>
       <c r="H85" s="50"/>
-      <c r="I85" s="51"/>
+      <c r="I85" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>REPROVADO</v>
+      </c>
       <c r="J85" s="52"/>
     </row>
     <row r="86" spans="2:10" x14ac:dyDescent="0.25">
@@ -2878,7 +3113,10 @@
         <v>125.42351427387632</v>
       </c>
       <c r="H86" s="50"/>
-      <c r="I86" s="51"/>
+      <c r="I86" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>REPROVADO</v>
+      </c>
       <c r="J86" s="52"/>
     </row>
     <row r="87" spans="2:10" x14ac:dyDescent="0.25">
@@ -2897,7 +3135,10 @@
         <v>118.41262355685092</v>
       </c>
       <c r="H87" s="50"/>
-      <c r="I87" s="51"/>
+      <c r="I87" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>RETRABALHO</v>
+      </c>
       <c r="J87" s="52"/>
     </row>
     <row r="88" spans="2:10" x14ac:dyDescent="0.25">
@@ -2916,7 +3157,10 @@
         <v>118.63619229741374</v>
       </c>
       <c r="H88" s="50"/>
-      <c r="I88" s="51"/>
+      <c r="I88" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>APROVADO</v>
+      </c>
       <c r="J88" s="52"/>
     </row>
     <row r="89" spans="2:10" x14ac:dyDescent="0.25">
@@ -2935,7 +3179,10 @@
         <v>119.75253501688984</v>
       </c>
       <c r="H89" s="50"/>
-      <c r="I89" s="51"/>
+      <c r="I89" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>APROVADO</v>
+      </c>
       <c r="J89" s="52"/>
     </row>
     <row r="90" spans="2:10" x14ac:dyDescent="0.25">
@@ -2954,7 +3201,10 @@
         <v>121.91259546307042</v>
       </c>
       <c r="H90" s="50"/>
-      <c r="I90" s="51"/>
+      <c r="I90" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>REPROVADO</v>
+      </c>
       <c r="J90" s="52"/>
     </row>
     <row r="91" spans="2:10" x14ac:dyDescent="0.25">
@@ -2973,7 +3223,10 @@
         <v>121.65947293426213</v>
       </c>
       <c r="H91" s="50"/>
-      <c r="I91" s="51"/>
+      <c r="I91" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>REPROVADO</v>
+      </c>
       <c r="J91" s="52"/>
     </row>
     <row r="92" spans="2:10" x14ac:dyDescent="0.25">
@@ -2992,7 +3245,10 @@
         <v>125.95784384361819</v>
       </c>
       <c r="H92" s="50"/>
-      <c r="I92" s="51"/>
+      <c r="I92" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>REPROVADO</v>
+      </c>
       <c r="J92" s="52"/>
     </row>
     <row r="93" spans="2:10" x14ac:dyDescent="0.25">
@@ -3011,7 +3267,10 @@
         <v>119.00514310188093</v>
       </c>
       <c r="H93" s="50"/>
-      <c r="I93" s="51"/>
+      <c r="I93" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>APROVADO</v>
+      </c>
       <c r="J93" s="52"/>
     </row>
     <row r="94" spans="2:10" x14ac:dyDescent="0.25">
@@ -3030,7 +3289,10 @@
         <v>125.85456070310903</v>
       </c>
       <c r="H94" s="50"/>
-      <c r="I94" s="51"/>
+      <c r="I94" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>REPROVADO</v>
+      </c>
       <c r="J94" s="52"/>
     </row>
     <row r="95" spans="2:10" x14ac:dyDescent="0.25">
@@ -3049,7 +3311,10 @@
         <v>122.19079938377845</v>
       </c>
       <c r="H95" s="50"/>
-      <c r="I95" s="51"/>
+      <c r="I95" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>REPROVADO</v>
+      </c>
       <c r="J95" s="52"/>
     </row>
     <row r="96" spans="2:10" x14ac:dyDescent="0.25">
@@ -3068,7 +3333,10 @@
         <v>119.08497111614902</v>
       </c>
       <c r="H96" s="50"/>
-      <c r="I96" s="51"/>
+      <c r="I96" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>APROVADO</v>
+      </c>
       <c r="J96" s="52"/>
     </row>
     <row r="97" spans="2:10" x14ac:dyDescent="0.25">
@@ -3087,7 +3355,10 @@
         <v>125.48151067087353</v>
       </c>
       <c r="H97" s="50"/>
-      <c r="I97" s="51"/>
+      <c r="I97" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>REPROVADO</v>
+      </c>
       <c r="J97" s="52"/>
     </row>
     <row r="98" spans="2:10" x14ac:dyDescent="0.25">
@@ -3106,7 +3377,10 @@
         <v>119.65376332168178</v>
       </c>
       <c r="H98" s="50"/>
-      <c r="I98" s="51"/>
+      <c r="I98" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>APROVADO</v>
+      </c>
       <c r="J98" s="52"/>
     </row>
     <row r="99" spans="2:10" x14ac:dyDescent="0.25">
@@ -3125,7 +3399,10 @@
         <v>120.41588986731095</v>
       </c>
       <c r="H99" s="50"/>
-      <c r="I99" s="51"/>
+      <c r="I99" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>APROVADO</v>
+      </c>
       <c r="J99" s="52"/>
     </row>
     <row r="100" spans="2:10" x14ac:dyDescent="0.25">
@@ -3144,7 +3421,10 @@
         <v>118.49699891840332</v>
       </c>
       <c r="H100" s="50"/>
-      <c r="I100" s="51"/>
+      <c r="I100" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>RETRABALHO</v>
+      </c>
       <c r="J100" s="52"/>
     </row>
     <row r="101" spans="2:10" x14ac:dyDescent="0.25">
@@ -3163,7 +3443,10 @@
         <v>125.55073979785814</v>
       </c>
       <c r="H101" s="50"/>
-      <c r="I101" s="51"/>
+      <c r="I101" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>REPROVADO</v>
+      </c>
       <c r="J101" s="52"/>
     </row>
     <row r="102" spans="2:10" x14ac:dyDescent="0.25">
@@ -3182,7 +3465,10 @@
         <v>124.54011363958584</v>
       </c>
       <c r="H102" s="50"/>
-      <c r="I102" s="51"/>
+      <c r="I102" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>REPROVADO</v>
+      </c>
       <c r="J102" s="52"/>
     </row>
     <row r="103" spans="2:10" x14ac:dyDescent="0.25">
@@ -3201,7 +3487,10 @@
         <v>125.82416755739079</v>
       </c>
       <c r="H103" s="50"/>
-      <c r="I103" s="51"/>
+      <c r="I103" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>REPROVADO</v>
+      </c>
       <c r="J103" s="52"/>
     </row>
     <row r="104" spans="2:10" x14ac:dyDescent="0.25">
@@ -3220,7 +3509,10 @@
         <v>122.14533992575758</v>
       </c>
       <c r="H104" s="50"/>
-      <c r="I104" s="51"/>
+      <c r="I104" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>REPROVADO</v>
+      </c>
       <c r="J104" s="52"/>
     </row>
     <row r="105" spans="2:10" x14ac:dyDescent="0.25">
@@ -3239,7 +3531,10 @@
         <v>120.03399074134326</v>
       </c>
       <c r="H105" s="50"/>
-      <c r="I105" s="51"/>
+      <c r="I105" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>APROVADO</v>
+      </c>
       <c r="J105" s="52"/>
     </row>
     <row r="106" spans="2:10" x14ac:dyDescent="0.25">
@@ -3258,7 +3553,10 @@
         <v>119.40068700031406</v>
       </c>
       <c r="H106" s="50"/>
-      <c r="I106" s="51"/>
+      <c r="I106" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>APROVADO</v>
+      </c>
       <c r="J106" s="52"/>
     </row>
     <row r="107" spans="2:10" x14ac:dyDescent="0.25">
@@ -3277,7 +3575,10 @@
         <v>125.88760389492099</v>
       </c>
       <c r="H107" s="50"/>
-      <c r="I107" s="51"/>
+      <c r="I107" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>REPROVADO</v>
+      </c>
       <c r="J107" s="52"/>
     </row>
     <row r="108" spans="2:10" x14ac:dyDescent="0.25">
@@ -3296,7 +3597,10 @@
         <v>120.91349894276721</v>
       </c>
       <c r="H108" s="50"/>
-      <c r="I108" s="51"/>
+      <c r="I108" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>APROVADO</v>
+      </c>
       <c r="J108" s="52"/>
     </row>
     <row r="109" spans="2:10" x14ac:dyDescent="0.25">
@@ -3315,7 +3619,10 @@
         <v>118.56429553536229</v>
       </c>
       <c r="H109" s="50"/>
-      <c r="I109" s="51"/>
+      <c r="I109" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>APROVADO</v>
+      </c>
       <c r="J109" s="52"/>
     </row>
     <row r="110" spans="2:10" x14ac:dyDescent="0.25">
@@ -3334,7 +3641,10 @@
         <v>122.29729938133109</v>
       </c>
       <c r="H110" s="50"/>
-      <c r="I110" s="51"/>
+      <c r="I110" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>REPROVADO</v>
+      </c>
       <c r="J110" s="52"/>
     </row>
     <row r="111" spans="2:10" x14ac:dyDescent="0.25">
@@ -3353,7 +3663,10 @@
         <v>120.08744535651181</v>
       </c>
       <c r="H111" s="50"/>
-      <c r="I111" s="51"/>
+      <c r="I111" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>APROVADO</v>
+      </c>
       <c r="J111" s="52"/>
     </row>
     <row r="112" spans="2:10" x14ac:dyDescent="0.25">
@@ -3372,7 +3685,10 @@
         <v>122.15555100106941</v>
       </c>
       <c r="H112" s="50"/>
-      <c r="I112" s="51"/>
+      <c r="I112" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>REPROVADO</v>
+      </c>
       <c r="J112" s="52"/>
     </row>
     <row r="113" spans="2:10" x14ac:dyDescent="0.25">
@@ -3391,7 +3707,10 @@
         <v>124.51836626271557</v>
       </c>
       <c r="H113" s="50"/>
-      <c r="I113" s="51"/>
+      <c r="I113" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>REPROVADO</v>
+      </c>
       <c r="J113" s="52"/>
     </row>
     <row r="114" spans="2:10" x14ac:dyDescent="0.25">
@@ -3410,7 +3729,10 @@
         <v>122.76417366198649</v>
       </c>
       <c r="H114" s="50"/>
-      <c r="I114" s="51"/>
+      <c r="I114" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>REPROVADO</v>
+      </c>
       <c r="J114" s="52"/>
     </row>
     <row r="115" spans="2:10" x14ac:dyDescent="0.25">
@@ -3429,7 +3751,10 @@
         <v>125.25926657238509</v>
       </c>
       <c r="H115" s="50"/>
-      <c r="I115" s="51"/>
+      <c r="I115" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>REPROVADO</v>
+      </c>
       <c r="J115" s="52"/>
     </row>
     <row r="116" spans="2:10" x14ac:dyDescent="0.25">
@@ -3448,7 +3773,10 @@
         <v>122.45518382033362</v>
       </c>
       <c r="H116" s="50"/>
-      <c r="I116" s="51"/>
+      <c r="I116" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>REPROVADO</v>
+      </c>
       <c r="J116" s="52"/>
     </row>
     <row r="117" spans="2:10" x14ac:dyDescent="0.25">
@@ -3467,7 +3795,10 @@
         <v>122.65176799349119</v>
       </c>
       <c r="H117" s="50"/>
-      <c r="I117" s="51"/>
+      <c r="I117" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>REPROVADO</v>
+      </c>
       <c r="J117" s="52"/>
     </row>
     <row r="118" spans="2:10" x14ac:dyDescent="0.25">
@@ -3486,7 +3817,10 @@
         <v>124.89417436698888</v>
       </c>
       <c r="H118" s="50"/>
-      <c r="I118" s="51"/>
+      <c r="I118" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>REPROVADO</v>
+      </c>
       <c r="J118" s="52"/>
     </row>
     <row r="119" spans="2:10" x14ac:dyDescent="0.25">
@@ -3505,7 +3839,10 @@
         <v>119.64910024824479</v>
       </c>
       <c r="H119" s="50"/>
-      <c r="I119" s="51"/>
+      <c r="I119" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>APROVADO</v>
+      </c>
       <c r="J119" s="52"/>
     </row>
     <row r="120" spans="2:10" x14ac:dyDescent="0.25">
@@ -3524,7 +3861,10 @@
         <v>119.8150178007716</v>
       </c>
       <c r="H120" s="50"/>
-      <c r="I120" s="51"/>
+      <c r="I120" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>APROVADO</v>
+      </c>
       <c r="J120" s="52"/>
     </row>
     <row r="121" spans="2:10" x14ac:dyDescent="0.25">
@@ -3543,7 +3883,10 @@
         <v>125.38797660852492</v>
       </c>
       <c r="H121" s="50"/>
-      <c r="I121" s="51"/>
+      <c r="I121" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>REPROVADO</v>
+      </c>
       <c r="J121" s="52"/>
     </row>
     <row r="122" spans="2:10" x14ac:dyDescent="0.25">
@@ -3562,7 +3905,10 @@
         <v>124.98116079901156</v>
       </c>
       <c r="H122" s="50"/>
-      <c r="I122" s="51"/>
+      <c r="I122" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>REPROVADO</v>
+      </c>
       <c r="J122" s="52"/>
     </row>
     <row r="123" spans="2:10" x14ac:dyDescent="0.25">
@@ -3581,7 +3927,10 @@
         <v>124.07909826817244</v>
       </c>
       <c r="H123" s="50"/>
-      <c r="I123" s="51"/>
+      <c r="I123" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>REPROVADO</v>
+      </c>
       <c r="J123" s="52"/>
     </row>
     <row r="124" spans="2:10" x14ac:dyDescent="0.25">
@@ -3600,7 +3949,10 @@
         <v>121.43093087387709</v>
       </c>
       <c r="H124" s="50"/>
-      <c r="I124" s="51"/>
+      <c r="I124" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>APROVADO</v>
+      </c>
       <c r="J124" s="52"/>
     </row>
     <row r="125" spans="2:10" x14ac:dyDescent="0.25">
@@ -3619,7 +3971,10 @@
         <v>119.85789661272406</v>
       </c>
       <c r="H125" s="50"/>
-      <c r="I125" s="51"/>
+      <c r="I125" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>APROVADO</v>
+      </c>
       <c r="J125" s="52"/>
     </row>
     <row r="126" spans="2:10" x14ac:dyDescent="0.25">
@@ -3638,7 +3993,10 @@
         <v>120.67835177341965</v>
       </c>
       <c r="H126" s="50"/>
-      <c r="I126" s="51"/>
+      <c r="I126" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>APROVADO</v>
+      </c>
       <c r="J126" s="52"/>
     </row>
     <row r="127" spans="2:10" x14ac:dyDescent="0.25">
@@ -3657,7 +4015,10 @@
         <v>123.78721643283997</v>
       </c>
       <c r="H127" s="50"/>
-      <c r="I127" s="51"/>
+      <c r="I127" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>REPROVADO</v>
+      </c>
       <c r="J127" s="52"/>
     </row>
     <row r="128" spans="2:10" x14ac:dyDescent="0.25">
@@ -3676,7 +4037,10 @@
         <v>120.24292803356593</v>
       </c>
       <c r="H128" s="50"/>
-      <c r="I128" s="51"/>
+      <c r="I128" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>APROVADO</v>
+      </c>
       <c r="J128" s="52"/>
     </row>
     <row r="129" spans="2:10" x14ac:dyDescent="0.25">
@@ -3695,7 +4059,10 @@
         <v>122.12177995931779</v>
       </c>
       <c r="H129" s="50"/>
-      <c r="I129" s="51"/>
+      <c r="I129" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>REPROVADO</v>
+      </c>
       <c r="J129" s="52"/>
     </row>
     <row r="130" spans="2:10" x14ac:dyDescent="0.25">
@@ -3714,7 +4081,10 @@
         <v>125.62269999949515</v>
       </c>
       <c r="H130" s="50"/>
-      <c r="I130" s="51"/>
+      <c r="I130" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>REPROVADO</v>
+      </c>
       <c r="J130" s="52"/>
     </row>
     <row r="131" spans="2:10" x14ac:dyDescent="0.25">
@@ -3733,7 +4103,10 @@
         <v>119.93722816923059</v>
       </c>
       <c r="H131" s="50"/>
-      <c r="I131" s="51"/>
+      <c r="I131" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>APROVADO</v>
+      </c>
       <c r="J131" s="52"/>
     </row>
     <row r="132" spans="2:10" x14ac:dyDescent="0.25">
@@ -3752,7 +4125,10 @@
         <v>122.24214128700177</v>
       </c>
       <c r="H132" s="50"/>
-      <c r="I132" s="51"/>
+      <c r="I132" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>REPROVADO</v>
+      </c>
       <c r="J132" s="52"/>
     </row>
     <row r="133" spans="2:10" x14ac:dyDescent="0.25">
@@ -3771,7 +4147,10 @@
         <v>122.48794558829741</v>
       </c>
       <c r="H133" s="50"/>
-      <c r="I133" s="51"/>
+      <c r="I133" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>REPROVADO</v>
+      </c>
       <c r="J133" s="52"/>
     </row>
     <row r="134" spans="2:10" x14ac:dyDescent="0.25">
@@ -3790,7 +4169,10 @@
         <v>118.17687469335456</v>
       </c>
       <c r="H134" s="50"/>
-      <c r="I134" s="51"/>
+      <c r="I134" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>RETRABALHO</v>
+      </c>
       <c r="J134" s="52"/>
     </row>
     <row r="135" spans="2:10" x14ac:dyDescent="0.25">
@@ -3809,7 +4191,10 @@
         <v>123.77149534849298</v>
       </c>
       <c r="H135" s="50"/>
-      <c r="I135" s="51"/>
+      <c r="I135" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>REPROVADO</v>
+      </c>
       <c r="J135" s="52"/>
     </row>
     <row r="136" spans="2:10" x14ac:dyDescent="0.25">
@@ -3828,7 +4213,10 @@
         <v>118.39222535560845</v>
       </c>
       <c r="H136" s="50"/>
-      <c r="I136" s="51"/>
+      <c r="I136" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>RETRABALHO</v>
+      </c>
       <c r="J136" s="52"/>
     </row>
     <row r="137" spans="2:10" x14ac:dyDescent="0.25">
@@ -3847,7 +4235,10 @@
         <v>121.07319198223733</v>
       </c>
       <c r="H137" s="50"/>
-      <c r="I137" s="51"/>
+      <c r="I137" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>APROVADO</v>
+      </c>
       <c r="J137" s="52"/>
     </row>
     <row r="138" spans="2:10" x14ac:dyDescent="0.25">
@@ -3866,7 +4257,10 @@
         <v>120.7375667733654</v>
       </c>
       <c r="H138" s="50"/>
-      <c r="I138" s="51"/>
+      <c r="I138" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>APROVADO</v>
+      </c>
       <c r="J138" s="52"/>
     </row>
   </sheetData>
@@ -4378,7 +4772,7 @@
       <formula>"Reprovado"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
-      <formula>"Aprovada"</formula>
+      <formula>"Aprovado"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>